<commit_message>
/update example adding 2 outputs of  one process
</commit_message>
<xml_diff>
--- a/config/MasterTable.xlsx
+++ b/config/MasterTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="10905" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="12105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
   <si>
     <t>TAG</t>
   </si>
@@ -132,6 +132,21 @@
   </si>
   <si>
     <t>FEATURES_NAMES</t>
+  </si>
+  <si>
+    <t>O7</t>
+  </si>
+  <si>
+    <t>TANK1</t>
+  </si>
+  <si>
+    <t>Variable de entrada al proceso tanque TANK1. No es una variable de decisión del optimizador. Variable Observada. Es un ejemplo de un flujo constante de entrada</t>
+  </si>
+  <si>
+    <t>Variable target del proceso B que finaliza el proceso</t>
+  </si>
+  <si>
+    <t>Y3</t>
   </si>
 </sst>
 </file>
@@ -476,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,7 +673,7 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
         <v>29</v>
@@ -667,7 +682,7 @@
         <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -690,63 +705,103 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>30</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>11</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>17</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C14" t="s">
         <v>23</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D14" t="s">
         <v>28</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E14" t="s">
         <v>8</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
         <v>26</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D15" t="s">
         <v>29</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E15" t="s">
         <v>9</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F15" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
jo/corrections and created all configurtions tables for optimizer
</commit_message>
<xml_diff>
--- a/config/MasterTable.xlsx
+++ b/config/MasterTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="13305" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
   <si>
     <t>TAG</t>
   </si>
@@ -113,18 +113,6 @@
   </si>
   <si>
     <t>USE_ACTUAL_MODEL</t>
-  </si>
-  <si>
-    <t>MLA</t>
-  </si>
-  <si>
-    <t>MLB</t>
-  </si>
-  <si>
-    <t>MLB/MLC</t>
-  </si>
-  <si>
-    <t>MLC</t>
   </si>
   <si>
     <t xml:space="preserve">Variable target del proceso B y proceso C (y variable de entrada al tanque de la etapa siguiente si es existe y si es que es necesaria)
@@ -137,9 +125,6 @@
     <t>O7</t>
   </si>
   <si>
-    <t>TANK1</t>
-  </si>
-  <si>
     <t>Variable de entrada al proceso tanque TANK1. No es una variable de decisión del optimizador. Variable Observada. Es un ejemplo de un flujo constante de entrada</t>
   </si>
   <si>
@@ -147,6 +132,27 @@
   </si>
   <si>
     <t>Y3</t>
+  </si>
+  <si>
+    <t>PR_A_Y1</t>
+  </si>
+  <si>
+    <t>TK_1</t>
+  </si>
+  <si>
+    <t>PR_B_Y2</t>
+  </si>
+  <si>
+    <t>PR_B_Y2/PR_B_Y3</t>
+  </si>
+  <si>
+    <t>PR_C_Y2</t>
+  </si>
+  <si>
+    <t>PR_B_Y3</t>
+  </si>
+  <si>
+    <t>PR_B_Y2/PR_C_Y2</t>
   </si>
 </sst>
 </file>
@@ -493,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,7 +516,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -542,7 +548,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -562,7 +568,7 @@
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -582,7 +588,7 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -602,7 +608,7 @@
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -622,67 +628,67 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -702,7 +708,7 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -722,7 +728,7 @@
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="105" x14ac:dyDescent="0.25">
@@ -733,7 +739,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
         <v>30</v>
@@ -742,18 +748,18 @@
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
         <v>30</v>
@@ -762,7 +768,7 @@
         <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -782,15 +788,15 @@
         <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
@@ -802,7 +808,7 @@
         <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ji/update debbuging errors codes
</commit_message>
<xml_diff>
--- a/config/MasterTable.xlsx
+++ b/config/MasterTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="13305" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="13905" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>